<commit_message>
bikin biar ga ada duplikat masuk di tamu
</commit_message>
<xml_diff>
--- a/FIX_Data Tamu Dummy.xlsx
+++ b/FIX_Data Tamu Dummy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zahira\Documents\1 STIS\STIS smt 5\1 Project RPL\STIS-GRAD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B12FF822-D453-4AE2-A362-817C04AA9F0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E828A1A-9A3A-416B-A5E9-60180207B3D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="1080" windowWidth="17280" windowHeight="10536" xr2:uid="{D7013B3A-F570-4141-A3BD-51F8F682F655}"/>
+    <workbookView xWindow="732" yWindow="732" windowWidth="17280" windowHeight="10536" xr2:uid="{D7013B3A-F570-4141-A3BD-51F8F682F655}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="93">
   <si>
     <t>Nama</t>
   </si>
@@ -268,6 +268,51 @@
   </si>
   <si>
     <t>Badan Perencanaan Pembangunan Daerah</t>
+  </si>
+  <si>
+    <t>Lukman Hakim</t>
+  </si>
+  <si>
+    <t>lukman.hakim@travelindo.com</t>
+  </si>
+  <si>
+    <t>PT Travel Indo Raya</t>
+  </si>
+  <si>
+    <t>Dewi Sartika</t>
+  </si>
+  <si>
+    <t>dewi.sartika@poltek-x.ac.id</t>
+  </si>
+  <si>
+    <t>Politeknik Negeri X</t>
+  </si>
+  <si>
+    <t>Rio Ferdinand</t>
+  </si>
+  <si>
+    <t>rio.ferdinand@kesehatandaerah.go.id</t>
+  </si>
+  <si>
+    <t>Dinas Kesehatan Provinsi</t>
+  </si>
+  <si>
+    <t>Cindy Aurelia</t>
+  </si>
+  <si>
+    <t>cindy.aurelia@fashionista.net</t>
+  </si>
+  <si>
+    <t>Aurelia Fashion Group</t>
+  </si>
+  <si>
+    <t>Haikal Zulkarnain</t>
+  </si>
+  <si>
+    <t>haikal.zul@softwareid.com</t>
+  </si>
+  <si>
+    <t>ID Software Development</t>
   </si>
 </sst>
 </file>
@@ -331,15 +376,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -654,17 +698,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7F7DF38-42B8-474E-A92F-E1D6C9A6E413}">
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C1048576"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.88671875" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.5546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="40.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -953,6 +997,61 @@
         <v>77</v>
       </c>
     </row>
+    <row r="27" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>